<commit_message>
fitting to data working
</commit_message>
<xml_diff>
--- a/data/230623_Kinetics_DA/output.xlsx
+++ b/data/230623_Kinetics_DA/output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Alba\Documents\GitHub\ECFERS\data\230623_Kinetics_DA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4966A1F9-EA2A-4D08-A166-D1A4102515DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DBABFB-1946-48C1-8938-AE7BF81ACC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="1935" windowWidth="37605" windowHeight="16725" xr2:uid="{B7E67C64-D74D-204A-861E-6D7F53143D6F}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{B7E67C64-D74D-204A-861E-6D7F53143D6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="286">
   <si>
     <t>Time</t>
   </si>
@@ -197,9 +197,6 @@
     <t>11175.44</t>
   </si>
   <si>
-    <t>15687.81</t>
-  </si>
-  <si>
     <t>14407.25</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>2384691.01</t>
   </si>
   <si>
-    <t>19816.11</t>
-  </si>
-  <si>
     <t>13270.59</t>
   </si>
   <si>
@@ -305,9 +299,6 @@
     <t>18062.61</t>
   </si>
   <si>
-    <t>15426.99</t>
-  </si>
-  <si>
     <t>10541.61</t>
   </si>
   <si>
@@ -383,18 +374,12 @@
     <t>1824050.95</t>
   </si>
   <si>
-    <t>35087.54</t>
-  </si>
-  <si>
     <t>1987637.50</t>
   </si>
   <si>
     <t>1468153.28</t>
   </si>
   <si>
-    <t>452673.46</t>
-  </si>
-  <si>
     <t>2575508.02</t>
   </si>
   <si>
@@ -407,9 +392,6 @@
     <t>12949.67</t>
   </si>
   <si>
-    <t>29579.07</t>
-  </si>
-  <si>
     <t>35884.95</t>
   </si>
   <si>
@@ -569,268 +551,349 @@
     <t>821794.12</t>
   </si>
   <si>
-    <t>404507.03</t>
-  </si>
-  <si>
-    <t>408382.39</t>
-  </si>
-  <si>
-    <t>281992.70</t>
-  </si>
-  <si>
-    <t>268142.11</t>
-  </si>
-  <si>
-    <t>237828.51</t>
-  </si>
-  <si>
-    <t>243362.92</t>
-  </si>
-  <si>
-    <t>215709.18</t>
-  </si>
-  <si>
-    <t>215544.64</t>
-  </si>
-  <si>
-    <t>260341.28</t>
-  </si>
-  <si>
-    <t>284048.10</t>
-  </si>
-  <si>
-    <t>452704.71</t>
-  </si>
-  <si>
-    <t>12251.59</t>
-  </si>
-  <si>
-    <t>459407.80</t>
-  </si>
-  <si>
-    <t>18334.31</t>
-  </si>
-  <si>
-    <t>1460.23</t>
-  </si>
-  <si>
-    <t>3958.76</t>
-  </si>
-  <si>
-    <t>13120.59</t>
-  </si>
-  <si>
-    <t>3261.90</t>
-  </si>
-  <si>
-    <t>12264.82</t>
-  </si>
-  <si>
-    <t>9164.35</t>
-  </si>
-  <si>
-    <t>3033.28</t>
-  </si>
-  <si>
-    <t>8929.85</t>
-  </si>
-  <si>
-    <t>10977.84</t>
-  </si>
-  <si>
-    <t>2427.06</t>
-  </si>
-  <si>
-    <t>10826.19</t>
-  </si>
-  <si>
-    <t>10667.99</t>
-  </si>
-  <si>
-    <t>2969.52</t>
-  </si>
-  <si>
-    <t>11632.38</t>
-  </si>
-  <si>
-    <t>21726.70</t>
-  </si>
-  <si>
-    <t>5799.50</t>
-  </si>
-  <si>
-    <t>19645.88</t>
-  </si>
-  <si>
-    <t>5258.27</t>
-  </si>
-  <si>
-    <t>4952.51</t>
-  </si>
-  <si>
-    <t>4091.68</t>
-  </si>
-  <si>
-    <t>1844.20</t>
-  </si>
-  <si>
-    <t>1322.99</t>
-  </si>
-  <si>
-    <t>1796.23</t>
-  </si>
-  <si>
-    <t>3702.38</t>
-  </si>
-  <si>
-    <t>3186.01</t>
-  </si>
-  <si>
-    <t>5134.84</t>
-  </si>
-  <si>
-    <t>5310.47</t>
-  </si>
-  <si>
-    <t>4987.11</t>
-  </si>
-  <si>
-    <t>3286.74</t>
-  </si>
-  <si>
-    <t>3450.75</t>
-  </si>
-  <si>
-    <t>3369.07</t>
-  </si>
-  <si>
-    <t>2125.14</t>
-  </si>
-  <si>
-    <t>3348.10</t>
-  </si>
-  <si>
-    <t>3277.26</t>
-  </si>
-  <si>
-    <t>4287.20</t>
-  </si>
-  <si>
-    <t>4979.17</t>
-  </si>
-  <si>
-    <t>1453.02</t>
-  </si>
-  <si>
-    <t>2721.04</t>
-  </si>
-  <si>
-    <t>1851.01</t>
-  </si>
-  <si>
-    <t>2517.18</t>
-  </si>
-  <si>
-    <t>2663.08</t>
-  </si>
-  <si>
-    <t>3561.55</t>
-  </si>
-  <si>
-    <t>5249.30</t>
-  </si>
-  <si>
-    <t>6282.65</t>
-  </si>
-  <si>
-    <t>3714.73</t>
-  </si>
-  <si>
-    <t>3959.24</t>
-  </si>
-  <si>
-    <t>1676.93</t>
-  </si>
-  <si>
-    <t>2625.96</t>
-  </si>
-  <si>
-    <t>2410.30</t>
-  </si>
-  <si>
-    <t>4080.58</t>
-  </si>
-  <si>
-    <t>4187.89</t>
-  </si>
-  <si>
-    <t>7362.04</t>
-  </si>
-  <si>
-    <t>6239.05</t>
-  </si>
-  <si>
-    <t>2960.51</t>
-  </si>
-  <si>
-    <t>2025.53</t>
-  </si>
-  <si>
-    <t>2849.61</t>
-  </si>
-  <si>
-    <t>2619.93</t>
-  </si>
-  <si>
-    <t>1520.20</t>
-  </si>
-  <si>
-    <t>4757.36</t>
-  </si>
-  <si>
-    <t>3588.22</t>
-  </si>
-  <si>
-    <t>2480.48</t>
-  </si>
-  <si>
-    <t>1296.50</t>
-  </si>
-  <si>
-    <t>1416.40</t>
-  </si>
-  <si>
-    <t>3163.86</t>
-  </si>
-  <si>
-    <t>2839.76</t>
-  </si>
-  <si>
-    <t>1312.82</t>
-  </si>
-  <si>
-    <t>1616.87</t>
-  </si>
-  <si>
-    <t>1003.93</t>
-  </si>
-  <si>
-    <t>2244.29</t>
-  </si>
-  <si>
-    <t>1219.93</t>
-  </si>
-  <si>
-    <t>1037.16</t>
-  </si>
-  <si>
-    <t>1462.34</t>
-  </si>
-  <si>
-    <t>2645.84</t>
-  </si>
-  <si>
-    <t>4080.73</t>
+    <t>1647767.38</t>
+  </si>
+  <si>
+    <t>1980057.98</t>
+  </si>
+  <si>
+    <t>387192.52</t>
+  </si>
+  <si>
+    <t>1693836.00</t>
+  </si>
+  <si>
+    <t>910960.99</t>
+  </si>
+  <si>
+    <t>1223425.31</t>
+  </si>
+  <si>
+    <t>867101.06</t>
+  </si>
+  <si>
+    <t>1165810.34</t>
+  </si>
+  <si>
+    <t>772065.24</t>
+  </si>
+  <si>
+    <t>1074006.65</t>
+  </si>
+  <si>
+    <t>1390646.14</t>
+  </si>
+  <si>
+    <t>1505026.93</t>
+  </si>
+  <si>
+    <t>Glyoxylate_Rep1</t>
+  </si>
+  <si>
+    <t>Glyoxylate_Rep2</t>
+  </si>
+  <si>
+    <t>Glyoxylate_Rep3</t>
+  </si>
+  <si>
+    <t>Citrate_Rep1</t>
+  </si>
+  <si>
+    <t>Citrate_Rep2</t>
+  </si>
+  <si>
+    <t>Citrate_Rep3</t>
+  </si>
+  <si>
+    <t>Fumerate_Rep1</t>
+  </si>
+  <si>
+    <t>Fumerate_Rep2</t>
+  </si>
+  <si>
+    <t>609680.38</t>
+  </si>
+  <si>
+    <t>900541.18</t>
+  </si>
+  <si>
+    <t>1778753.36</t>
+  </si>
+  <si>
+    <t>1642028.42</t>
+  </si>
+  <si>
+    <t>1726556.88</t>
+  </si>
+  <si>
+    <t>1755879.43</t>
+  </si>
+  <si>
+    <t>1852497.85</t>
+  </si>
+  <si>
+    <t>1611529.1</t>
+  </si>
+  <si>
+    <t>1705032.07</t>
+  </si>
+  <si>
+    <t>1479060.02</t>
+  </si>
+  <si>
+    <t>1752621.51</t>
+  </si>
+  <si>
+    <t>1867726.97</t>
+  </si>
+  <si>
+    <t>52057.86</t>
+  </si>
+  <si>
+    <t>54413.12</t>
+  </si>
+  <si>
+    <t>62310.72</t>
+  </si>
+  <si>
+    <t>418213</t>
+  </si>
+  <si>
+    <t>461977</t>
+  </si>
+  <si>
+    <t>249503</t>
+  </si>
+  <si>
+    <t>114952</t>
+  </si>
+  <si>
+    <t>117630</t>
+  </si>
+  <si>
+    <t>439223</t>
+  </si>
+  <si>
+    <t>412081</t>
+  </si>
+  <si>
+    <t>188424</t>
+  </si>
+  <si>
+    <t>159081</t>
+  </si>
+  <si>
+    <t>160629</t>
+  </si>
+  <si>
+    <t>152746</t>
+  </si>
+  <si>
+    <t>409591</t>
+  </si>
+  <si>
+    <t>405507</t>
+  </si>
+  <si>
+    <t>123998</t>
+  </si>
+  <si>
+    <t>118261</t>
+  </si>
+  <si>
+    <t>132296</t>
+  </si>
+  <si>
+    <t>113890</t>
+  </si>
+  <si>
+    <t>516867</t>
+  </si>
+  <si>
+    <t>645508</t>
+  </si>
+  <si>
+    <t>80133</t>
+  </si>
+  <si>
+    <t>100613</t>
+  </si>
+  <si>
+    <t>849370</t>
+  </si>
+  <si>
+    <t>856524</t>
+  </si>
+  <si>
+    <t>189425</t>
+  </si>
+  <si>
+    <t>22196</t>
+  </si>
+  <si>
+    <t>30695</t>
+  </si>
+  <si>
+    <t>47354</t>
+  </si>
+  <si>
+    <t>72036</t>
+  </si>
+  <si>
+    <t>124763</t>
+  </si>
+  <si>
+    <t>105103</t>
+  </si>
+  <si>
+    <t>259472</t>
+  </si>
+  <si>
+    <t>189596</t>
+  </si>
+  <si>
+    <t>Fumerate_Rep3</t>
+  </si>
+  <si>
+    <t>244209</t>
+  </si>
+  <si>
+    <t>193530</t>
+  </si>
+  <si>
+    <t>113373</t>
+  </si>
+  <si>
+    <t>100486</t>
+  </si>
+  <si>
+    <t>297778</t>
+  </si>
+  <si>
+    <t>287321</t>
+  </si>
+  <si>
+    <t>5829142</t>
+  </si>
+  <si>
+    <t>4487696</t>
+  </si>
+  <si>
+    <t>5009484</t>
+  </si>
+  <si>
+    <t>4748367</t>
+  </si>
+  <si>
+    <t>4695993</t>
+  </si>
+  <si>
+    <t>4920358</t>
+  </si>
+  <si>
+    <t>4977307</t>
+  </si>
+  <si>
+    <t>4959463</t>
+  </si>
+  <si>
+    <t>4218076</t>
+  </si>
+  <si>
+    <t>5759889</t>
+  </si>
+  <si>
+    <t>4813094</t>
+  </si>
+  <si>
+    <t>779764</t>
+  </si>
+  <si>
+    <t>585855</t>
+  </si>
+  <si>
+    <t>592555</t>
+  </si>
+  <si>
+    <t>339089</t>
+  </si>
+  <si>
+    <t>331266</t>
+  </si>
+  <si>
+    <t>177654</t>
+  </si>
+  <si>
+    <t>409515</t>
+  </si>
+  <si>
+    <t>261917</t>
+  </si>
+  <si>
+    <t>517842</t>
+  </si>
+  <si>
+    <t>232698</t>
+  </si>
+  <si>
+    <t>625278</t>
+  </si>
+  <si>
+    <t>374094</t>
+  </si>
+  <si>
+    <t>225713</t>
+  </si>
+  <si>
+    <t>191147</t>
+  </si>
+  <si>
+    <t>49374</t>
+  </si>
+  <si>
+    <t>97863</t>
+  </si>
+  <si>
+    <t>87076</t>
+  </si>
+  <si>
+    <t>127753</t>
+  </si>
+  <si>
+    <t>99621</t>
+  </si>
+  <si>
+    <t>237960</t>
+  </si>
+  <si>
+    <t>241556</t>
+  </si>
+  <si>
+    <t>284466</t>
+  </si>
+  <si>
+    <t>248285</t>
+  </si>
+  <si>
+    <t>304759</t>
+  </si>
+  <si>
+    <t>206512</t>
+  </si>
+  <si>
+    <t>193139</t>
+  </si>
+  <si>
+    <t>213237</t>
+  </si>
+  <si>
+    <t>244665</t>
+  </si>
+  <si>
+    <t>239272</t>
+  </si>
+  <si>
+    <t>351372</t>
   </si>
 </sst>
 </file>
@@ -1203,16 +1266,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45EC61B-23EC-A443-9B2C-94C166603EF1}">
-  <dimension ref="A1:AU31"/>
+  <dimension ref="A1:BD31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AS20" sqref="AS20:AU20"/>
+      <pane xSplit="1" topLeftCell="AU1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BB31" sqref="BB31:BC31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1351,8 +1414,35 @@
       <c r="AU1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AV1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>187</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1369,34 +1459,31 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="P2" t="s">
-        <v>162</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>208</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>209</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>244</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>245</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="AY2">
+        <v>340322</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>206</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>236</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1413,28 +1500,25 @@
         <v>0.5</v>
       </c>
       <c r="I3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J3" t="s">
-        <v>88</v>
-      </c>
-      <c r="K3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>210</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>211</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>247</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>208</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>239</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1451,10 +1535,10 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1471,7 +1555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1488,19 +1572,19 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J6" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>212</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>241</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1522,29 +1606,32 @@
       <c r="G7" t="s">
         <v>52</v>
       </c>
-      <c r="H7" t="s">
-        <v>53</v>
-      </c>
       <c r="I7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P7" t="s">
-        <v>164</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>214</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>209</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>210</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>243</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1561,46 +1648,40 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
         <v>57</v>
       </c>
-      <c r="G8" t="s">
-        <v>58</v>
-      </c>
       <c r="I8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="O8" t="s">
-        <v>156</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>177</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>178</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>190</v>
-      </c>
-      <c r="AN8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AV8" t="s">
         <v>191</v>
       </c>
-      <c r="AO8" t="s">
+      <c r="AW8" t="s">
         <v>192</v>
       </c>
-      <c r="AS8" t="s">
-        <v>254</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>255</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AY8" t="s">
+        <v>211</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>212</v>
+      </c>
+      <c r="BB8">
+        <v>6013398</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1617,43 +1698,40 @@
         <v>0.5</v>
       </c>
       <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
         <v>63</v>
       </c>
-      <c r="G9" t="s">
-        <v>64</v>
-      </c>
       <c r="I9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O9" t="s">
-        <v>157</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>179</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>180</v>
-      </c>
-      <c r="AM9" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV9" t="s">
         <v>193</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AW9" t="s">
         <v>194</v>
       </c>
-      <c r="AO9" t="s">
-        <v>195</v>
-      </c>
-      <c r="AS9" t="s">
-        <v>257</v>
-      </c>
-      <c r="AT9" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AY9" t="s">
+        <v>213</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>214</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>246</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1670,34 +1748,31 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
         <v>67</v>
       </c>
-      <c r="G10" t="s">
-        <v>68</v>
-      </c>
       <c r="I10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>181</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>182</v>
-      </c>
-      <c r="AM10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW10" t="s">
         <v>196</v>
       </c>
-      <c r="AN10" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BB10" t="s">
+        <v>248</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1714,34 +1789,31 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" t="s">
         <v>59</v>
       </c>
-      <c r="G11" t="s">
-        <v>60</v>
-      </c>
       <c r="I11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J11" t="s">
-        <v>100</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>183</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>184</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>199</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>200</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>197</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>198</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>250</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1758,37 +1830,34 @@
         <v>4</v>
       </c>
       <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
         <v>61</v>
       </c>
-      <c r="G12" t="s">
-        <v>62</v>
-      </c>
       <c r="I12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="O12" t="s">
-        <v>158</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>185</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>186</v>
-      </c>
-      <c r="AM12" t="s">
-        <v>202</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>203</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>200</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>252</v>
+      </c>
+      <c r="BC12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1805,43 +1874,43 @@
         <v>8</v>
       </c>
       <c r="F13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
         <v>65</v>
       </c>
-      <c r="G13" t="s">
-        <v>66</v>
-      </c>
       <c r="I13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="O13" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="P13" t="s">
-        <v>160</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>187</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>188</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>189</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>205</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>206</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>202</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>215</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>216</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>254</v>
+      </c>
+      <c r="BC13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1858,34 +1927,37 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" t="s">
         <v>69</v>
       </c>
-      <c r="G14" t="s">
-        <v>70</v>
-      </c>
       <c r="I14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J14" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM14" t="s">
-        <v>233</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>234</v>
-      </c>
-      <c r="AS14" t="s">
-        <v>259</v>
-      </c>
-      <c r="AT14" t="s">
-        <v>260</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>203</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>204</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>217</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>218</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>256</v>
+      </c>
+      <c r="BC14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1902,28 +1974,34 @@
         <v>0.5</v>
       </c>
       <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" t="s">
         <v>71</v>
       </c>
-      <c r="G15" t="s">
-        <v>72</v>
-      </c>
       <c r="I15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="O15" t="s">
-        <v>154</v>
-      </c>
-      <c r="AM15" t="s">
-        <v>235</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>220</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>258</v>
+      </c>
+      <c r="BC15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1940,22 +2018,25 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" t="s">
         <v>73</v>
       </c>
-      <c r="G16" t="s">
-        <v>74</v>
-      </c>
       <c r="I16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J16" t="s">
-        <v>112</v>
-      </c>
-      <c r="AM16" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="BB16" t="s">
+        <v>260</v>
+      </c>
+      <c r="BC16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1972,28 +2053,25 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" t="s">
         <v>75</v>
       </c>
-      <c r="G17" t="s">
-        <v>76</v>
-      </c>
       <c r="I17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J17" t="s">
-        <v>114</v>
-      </c>
-      <c r="K17" t="s">
-        <v>115</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>238</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>262</v>
+      </c>
+      <c r="BC17" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2010,28 +2088,25 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" t="s">
         <v>77</v>
       </c>
-      <c r="G18" t="s">
-        <v>78</v>
-      </c>
       <c r="I18" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J18" t="s">
-        <v>117</v>
-      </c>
-      <c r="K18" t="s">
-        <v>118</v>
-      </c>
-      <c r="AM18" t="s">
-        <v>240</v>
-      </c>
-      <c r="AN18" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>264</v>
+      </c>
+      <c r="BC18" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2048,28 +2123,37 @@
         <v>8</v>
       </c>
       <c r="F19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" t="s">
         <v>79</v>
       </c>
-      <c r="G19" t="s">
-        <v>80</v>
-      </c>
       <c r="I19" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J19" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="O19" t="s">
-        <v>155</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>242</v>
-      </c>
-      <c r="AN19" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="AV19" t="s">
+        <v>205</v>
+      </c>
+      <c r="AY19" t="s">
+        <v>221</v>
+      </c>
+      <c r="AZ19" t="s">
+        <v>222</v>
+      </c>
+      <c r="BB19" t="s">
+        <v>266</v>
+      </c>
+      <c r="BC19" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2086,46 +2170,43 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" t="s">
         <v>81</v>
       </c>
-      <c r="G20" t="s">
-        <v>82</v>
-      </c>
-      <c r="H20" t="s">
-        <v>83</v>
-      </c>
       <c r="I20" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="J20" t="s">
-        <v>122</v>
-      </c>
-      <c r="K20" t="s">
-        <v>123</v>
+        <v>117</v>
+      </c>
+      <c r="L20" t="s">
+        <v>171</v>
+      </c>
+      <c r="M20" t="s">
+        <v>172</v>
       </c>
       <c r="O20" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="P20" t="s">
-        <v>143</v>
-      </c>
-      <c r="AM20" t="s">
-        <v>225</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>226</v>
-      </c>
-      <c r="AS20" t="s">
-        <v>262</v>
-      </c>
-      <c r="AT20" t="s">
-        <v>263</v>
-      </c>
-      <c r="AU20" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="AY20" t="s">
+        <v>223</v>
+      </c>
+      <c r="AZ20" t="s">
+        <v>224</v>
+      </c>
+      <c r="BB20" t="s">
+        <v>268</v>
+      </c>
+      <c r="BC20" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -2141,14 +2222,23 @@
       <c r="E21">
         <v>0.5</v>
       </c>
+      <c r="L21" t="s">
+        <v>173</v>
+      </c>
+      <c r="M21" t="s">
+        <v>174</v>
+      </c>
       <c r="O21" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="P21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="BB21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2164,14 +2254,20 @@
       <c r="E22">
         <v>1</v>
       </c>
+      <c r="L22" t="s">
+        <v>175</v>
+      </c>
+      <c r="M22" t="s">
+        <v>176</v>
+      </c>
       <c r="O22" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P22" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2188,25 +2284,31 @@
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J23" t="s">
-        <v>125</v>
+        <v>119</v>
+      </c>
+      <c r="L23" t="s">
+        <v>177</v>
+      </c>
+      <c r="M23" t="s">
+        <v>178</v>
       </c>
       <c r="O23" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="P23" t="s">
-        <v>149</v>
-      </c>
-      <c r="AM23" t="s">
-        <v>227</v>
-      </c>
-      <c r="AN23" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="BB23" t="s">
+        <v>271</v>
+      </c>
+      <c r="BC23" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2223,25 +2325,31 @@
         <v>4</v>
       </c>
       <c r="I24" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J24" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+      <c r="L24" t="s">
+        <v>179</v>
+      </c>
+      <c r="M24" t="s">
+        <v>180</v>
       </c>
       <c r="O24" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="P24" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM24" t="s">
-        <v>229</v>
-      </c>
-      <c r="AN24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="BB24" t="s">
+        <v>273</v>
+      </c>
+      <c r="BC24" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2258,28 +2366,40 @@
         <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I25" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>123</v>
+      </c>
+      <c r="L25" t="s">
+        <v>181</v>
+      </c>
+      <c r="M25" t="s">
+        <v>182</v>
       </c>
       <c r="O25" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="P25" t="s">
-        <v>153</v>
-      </c>
-      <c r="AM25" t="s">
-        <v>231</v>
-      </c>
-      <c r="AN25" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="AY25" t="s">
+        <v>225</v>
+      </c>
+      <c r="AZ25" t="s">
+        <v>226</v>
+      </c>
+      <c r="BB25" t="s">
+        <v>275</v>
+      </c>
+      <c r="BC25" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2296,40 +2416,37 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" t="s">
         <v>54</v>
       </c>
-      <c r="G26" t="s">
-        <v>55</v>
-      </c>
       <c r="I26" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J26" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="O26" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="P26" t="s">
-        <v>166</v>
-      </c>
-      <c r="AM26" t="s">
-        <v>216</v>
-      </c>
-      <c r="AN26" t="s">
-        <v>217</v>
-      </c>
-      <c r="AS26" t="s">
-        <v>249</v>
-      </c>
-      <c r="AT26" t="s">
-        <v>250</v>
-      </c>
-      <c r="AU26" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="AY26" t="s">
+        <v>227</v>
+      </c>
+      <c r="AZ26" t="s">
+        <v>228</v>
+      </c>
+      <c r="BB26" t="s">
+        <v>277</v>
+      </c>
+      <c r="BC26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2346,28 +2463,25 @@
         <v>0.5</v>
       </c>
       <c r="I27" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="J27" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="O27" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="P27" t="s">
-        <v>168</v>
-      </c>
-      <c r="AM27" t="s">
-        <v>218</v>
-      </c>
-      <c r="AS27" t="s">
-        <v>252</v>
-      </c>
-      <c r="AT27" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="AY27" t="s">
+        <v>229</v>
+      </c>
+      <c r="BB27" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2384,19 +2498,19 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="J28" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="O28" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="P28" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2413,28 +2527,34 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I29" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="J29" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="O29" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="P29" t="s">
-        <v>172</v>
-      </c>
-      <c r="AM29" t="s">
-        <v>219</v>
-      </c>
-      <c r="AN29" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="AY29" t="s">
+        <v>230</v>
+      </c>
+      <c r="AZ29" t="s">
+        <v>231</v>
+      </c>
+      <c r="BB29" t="s">
+        <v>280</v>
+      </c>
+      <c r="BC29" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2451,25 +2571,31 @@
         <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="J30" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="O30" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="P30" t="s">
-        <v>174</v>
-      </c>
-      <c r="AM30" t="s">
-        <v>221</v>
-      </c>
-      <c r="AN30" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="AY30" t="s">
+        <v>232</v>
+      </c>
+      <c r="AZ30" t="s">
+        <v>233</v>
+      </c>
+      <c r="BB30" t="s">
+        <v>282</v>
+      </c>
+      <c r="BC30" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2486,22 +2612,28 @@
         <v>8</v>
       </c>
       <c r="I31" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="J31" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="O31" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="P31" t="s">
-        <v>176</v>
-      </c>
-      <c r="AM31" t="s">
-        <v>223</v>
-      </c>
-      <c r="AN31" t="s">
-        <v>224</v>
+        <v>170</v>
+      </c>
+      <c r="AY31" t="s">
+        <v>234</v>
+      </c>
+      <c r="AZ31" t="s">
+        <v>235</v>
+      </c>
+      <c r="BB31" t="s">
+        <v>284</v>
+      </c>
+      <c r="BC31" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data to fit HCT, dilution
</commit_message>
<xml_diff>
--- a/data/230623_Kinetics_DA/output.xlsx
+++ b/data/230623_Kinetics_DA/output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Alba\Documents\GitHub\ECFERS\data\230623_Kinetics_DA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DBABFB-1946-48C1-8938-AE7BF81ACC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EFACD5-6F7F-4201-AC67-5D8978CC73B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{B7E67C64-D74D-204A-861E-6D7F53143D6F}"/>
+    <workbookView xWindow="17835" yWindow="1380" windowWidth="14685" windowHeight="16725" xr2:uid="{B7E67C64-D74D-204A-861E-6D7F53143D6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -605,12 +605,6 @@
     <t>Citrate_Rep3</t>
   </si>
   <si>
-    <t>Fumerate_Rep1</t>
-  </si>
-  <si>
-    <t>Fumerate_Rep2</t>
-  </si>
-  <si>
     <t>609680.38</t>
   </si>
   <si>
@@ -752,9 +746,6 @@
     <t>189596</t>
   </si>
   <si>
-    <t>Fumerate_Rep3</t>
-  </si>
-  <si>
     <t>244209</t>
   </si>
   <si>
@@ -894,6 +885,15 @@
   </si>
   <si>
     <t>351372</t>
+  </si>
+  <si>
+    <t>Fumarate_Rep2</t>
+  </si>
+  <si>
+    <t>Fumarate_Rep1</t>
+  </si>
+  <si>
+    <t>Fumarate_Rep3</t>
   </si>
 </sst>
 </file>
@@ -1269,8 +1269,8 @@
   <dimension ref="A1:BD31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BB31" sqref="BB31:BC31"/>
+      <pane xSplit="1" topLeftCell="AZ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BB1" sqref="BB1:BD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1433,13 +1433,13 @@
         <v>188</v>
       </c>
       <c r="BB1" t="s">
-        <v>189</v>
+        <v>284</v>
       </c>
       <c r="BC1" t="s">
-        <v>190</v>
+        <v>283</v>
       </c>
       <c r="BD1" t="s">
-        <v>238</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
@@ -1474,13 +1474,13 @@
         <v>340322</v>
       </c>
       <c r="AZ2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="BB2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="BC2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
@@ -1506,16 +1506,16 @@
         <v>86</v>
       </c>
       <c r="AY3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AZ3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="BB3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="BC3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
@@ -1578,10 +1578,10 @@
         <v>89</v>
       </c>
       <c r="BB6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="BC6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
@@ -1619,16 +1619,16 @@
         <v>158</v>
       </c>
       <c r="AY7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AZ7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="BB7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="BC7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
@@ -1663,22 +1663,22 @@
         <v>150</v>
       </c>
       <c r="AV8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AW8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AY8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="AZ8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="BB8">
         <v>6013398</v>
       </c>
       <c r="BC8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
@@ -1713,22 +1713,22 @@
         <v>151</v>
       </c>
       <c r="AV9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="AW9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AY9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AZ9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="BB9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="BC9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
@@ -1760,16 +1760,16 @@
         <v>95</v>
       </c>
       <c r="AV10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AW10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="BB10" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="BC10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
@@ -1801,16 +1801,16 @@
         <v>97</v>
       </c>
       <c r="AV11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AW11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="BB11" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="BC11" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
@@ -1845,16 +1845,16 @@
         <v>152</v>
       </c>
       <c r="AV12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AW12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="BB12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="BC12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.25">
@@ -1892,22 +1892,22 @@
         <v>154</v>
       </c>
       <c r="AV13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AW13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AY13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AZ13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="BB13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="BC13" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.25">
@@ -1939,22 +1939,22 @@
         <v>105</v>
       </c>
       <c r="AV14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AW14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AY14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AZ14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="BB14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="BC14" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
@@ -1989,16 +1989,16 @@
         <v>148</v>
       </c>
       <c r="AY15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AZ15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="BB15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="BC15" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.25">
@@ -2030,10 +2030,10 @@
         <v>109</v>
       </c>
       <c r="BB16" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="BC16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:55" x14ac:dyDescent="0.25">
@@ -2065,10 +2065,10 @@
         <v>111</v>
       </c>
       <c r="BB17" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="BC17" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:55" x14ac:dyDescent="0.25">
@@ -2100,10 +2100,10 @@
         <v>113</v>
       </c>
       <c r="BB18" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="BC18" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:55" x14ac:dyDescent="0.25">
@@ -2138,19 +2138,19 @@
         <v>149</v>
       </c>
       <c r="AV19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AY19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AZ19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="BB19" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="BC19" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.25">
@@ -2194,16 +2194,16 @@
         <v>137</v>
       </c>
       <c r="AY20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AZ20" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="BB20" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="BC20" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:55" x14ac:dyDescent="0.25">
@@ -2235,7 +2235,7 @@
         <v>139</v>
       </c>
       <c r="BB21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:55" x14ac:dyDescent="0.25">
@@ -2302,10 +2302,10 @@
         <v>143</v>
       </c>
       <c r="BB23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="BC23" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:55" x14ac:dyDescent="0.25">
@@ -2343,10 +2343,10 @@
         <v>145</v>
       </c>
       <c r="BB24" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="BC24" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:55" x14ac:dyDescent="0.25">
@@ -2387,16 +2387,16 @@
         <v>147</v>
       </c>
       <c r="AY25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AZ25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="BB25" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="BC25" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:55" x14ac:dyDescent="0.25">
@@ -2434,16 +2434,16 @@
         <v>160</v>
       </c>
       <c r="AY26" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AZ26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="BB26" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="BC26" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:55" x14ac:dyDescent="0.25">
@@ -2475,10 +2475,10 @@
         <v>162</v>
       </c>
       <c r="AY27" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BB27" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:55" x14ac:dyDescent="0.25">
@@ -2542,16 +2542,16 @@
         <v>166</v>
       </c>
       <c r="AY29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AZ29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="BB29" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="BC29" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:55" x14ac:dyDescent="0.25">
@@ -2583,16 +2583,16 @@
         <v>168</v>
       </c>
       <c r="AY30" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AZ30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="BB30" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="BC30" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:55" x14ac:dyDescent="0.25">
@@ -2624,16 +2624,16 @@
         <v>170</v>
       </c>
       <c r="AY31" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AZ31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="BB31" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="BC31" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>